<commit_message>
Working on paths / material related termlists
</commit_message>
<xml_diff>
--- a/testtable.xlsx
+++ b/testtable.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="import this" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -223,174 +223,177 @@
     <t xml:space="preserve">chance find</t>
   </si>
   <si>
+    <t xml:space="preserve">donor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr. X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abu Nusayr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">جرش</t>
+  </si>
+  <si>
+    <t xml:space="preserve">som other name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abu Nusayr_mega</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35.76663, 31.98603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">baths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some context</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bronze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sculpture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">figurine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drawing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reddish-Brown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">none</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chasing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#333</t>
+  </si>
+  <si>
+    <t xml:space="preserve">undetermined</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">corroded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">none remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greco-Roman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">late 1st mill. BC-early 1st mill. AD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1st cent. BC-1st cent. AD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 BC-100 AD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I-II Century A.D.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a bronze figurine of hepocrates (horus the child), the god of silence and secrecy who was usually depicted as a little body with a forefinger held to his lips- an egyptian gesture symbolising childhood which the greeks mistook for a hush for silence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no literature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تمثال برونزي لهاربوكريت عاري</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">العرض</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P.A.M.40.1552</t>
+  </si>
+  <si>
+    <t xml:space="preserve">شراء</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unknown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1940?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in inventory book kind of acquisition is "unknown" and the date as well. Hashem Khries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vessel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oil Lamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bronze oil lamp with shell-shaped lid and cub-shaped handle attached to the lid of the filler hole and to the body of the oil lamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">سراج برونزي بشكل حيوان وغطاءفتحة الزيت على شكل صدفة</t>
+  </si>
+  <si>
+    <t xml:space="preserve">showcase A26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.M.41.572</t>
+  </si>
+  <si>
+    <t xml:space="preserve">institution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">بيزنطي</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-VI Century A.D.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">عقد صغير من الذهب واللولو  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> الذهب</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P.A.M.41.578</t>
+  </si>
+  <si>
     <t xml:space="preserve">A.S.O.R</t>
   </si>
   <si>
-    <t xml:space="preserve">Mr. X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abu Nusayr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">جرش</t>
-  </si>
-  <si>
-    <t xml:space="preserve">som other name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abu Nusayr_mega</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35.76663, 31.98603</t>
-  </si>
-  <si>
-    <t xml:space="preserve">baths</t>
-  </si>
-  <si>
-    <t xml:space="preserve">some context</t>
-  </si>
-  <si>
-    <t xml:space="preserve">some remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">metal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bronze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sculpture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">figurine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">drawing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reddish-Brown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">none</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chasing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#333</t>
-  </si>
-  <si>
-    <t xml:space="preserve">undetermined</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">corroded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">none remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Greco-Roman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">late 1st mill. BC-early 1st mill. AD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1st cent. BC-1st cent. AD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100 BC-100 AD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I-II Century A.D.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a bronze figurine of hepocrates (horus the child), the god of silence and secrecy who was usually depicted as a little body with a forefinger held to his lips- an egyptian gesture symbolising childhood which the greeks mistook for a hush for silence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no literature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">تمثال برونزي لهاربوكريت عاري</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">العرض</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P.A.M.40.1552</t>
-  </si>
-  <si>
-    <t xml:space="preserve">شراء</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unknown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1940?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">in inventory book kind of acquisition is "unknown" and the date as well. Hashem Khries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vessel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oil Lamp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Complete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bronze oil lamp with shell-shaped lid and cub-shaped handle attached to the lid of the filler hole and to the body of the oil lamp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">سراج برونزي بشكل حيوان وغطاءفتحة الزيت على شكل صدفة</t>
-  </si>
-  <si>
-    <t xml:space="preserve">showcase A26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A.M.41.572</t>
-  </si>
-  <si>
-    <t xml:space="preserve">institution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">بيزنطي</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V-VI Century A.D.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">عقد صغير من الذهب واللولو  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> الذهب</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P.A.M.41.578</t>
-  </si>
-  <si>
     <t xml:space="preserve">Byzantine V-VI Century A.D.</t>
   </si>
   <si>
@@ -407,9 +410,6 @@
   </si>
   <si>
     <t xml:space="preserve">.pA.M.41.579</t>
-  </si>
-  <si>
-    <t xml:space="preserve">donor</t>
   </si>
   <si>
     <t xml:space="preserve">Abu Habil</t>
@@ -467,6 +467,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -488,6 +489,7 @@
       <color rgb="FF24272D"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -670,15 +672,15 @@
   </sheetPr>
   <dimension ref="A1:BK10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AR1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BF3" activeCellId="0" sqref="BF3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.42"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="2" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="15.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="15.96"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="20" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -1249,7 +1251,7 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="n">
@@ -1307,13 +1309,13 @@
       <c r="BB5" s="2"/>
       <c r="BC5" s="2"/>
       <c r="BD5" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="BE5" s="2"/>
       <c r="BF5" s="2"/>
       <c r="BG5" s="2"/>
       <c r="BH5" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="BI5" s="2" t="s">
         <v>121</v>
@@ -1334,7 +1336,7 @@
         <v>22</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>1</v>
@@ -1343,10 +1345,10 @@
         <v>66</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J6" s="2" t="n">
         <v>1929</v>
@@ -1364,10 +1366,10 @@
         <v>118</v>
       </c>
       <c r="BD6" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="BH6" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="BI6" s="2" t="s">
         <v>121</v>
@@ -1387,13 +1389,13 @@
         <v>23</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>129</v>
+        <v>67</v>
       </c>
       <c r="J7" s="2" t="n">
         <v>1929</v>
@@ -1414,7 +1416,7 @@
         <v>118</v>
       </c>
       <c r="BD7" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="BH7" s="2" t="s">
         <v>131</v>
@@ -1449,7 +1451,7 @@
         <v>133</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="n">
@@ -1543,7 +1545,7 @@
         <v>138</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="J9" s="2" t="n">
         <v>1929</v>
@@ -1590,7 +1592,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="J10" s="2" t="n">
         <v>1929</v>

</xml_diff>